<commit_message>
refactor: nova coluna 'TIPO'
Para identificar o valor sem precisar do contexto da planilha. Pode ser ÁREA, PRODUTIVIDADE ou PRODUÇÃO.
</commit_message>
<xml_diff>
--- a/Base de Dados/Dados Tratados/DEZEMBRO_2022.xlsx
+++ b/Base de Dados/Dados Tratados/DEZEMBRO_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\GitHub\Projeto-Painel-de-BI-Dados-Agricolas\Base de Dados\Dados Tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C6CB6-5F9C-42FE-AF5B-11DF92442085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311CE6FC-7D8C-46F8-82E1-9E3DA8F7886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="70">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -240,6 +240,18 @@
   <si>
     <t>DEZEMBRO</t>
   </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>ÁREA</t>
+  </si>
+  <si>
+    <t>PRODUTIVIDADE</t>
+  </si>
+  <si>
+    <t>PRODUÇÃO</t>
+  </si>
 </sst>
 </file>
 
@@ -288,7 +300,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="193">
+  <dxfs count="197">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -360,12 +390,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -882,255 +906,261 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}" name="AREA_POR_PRODUTO" displayName="AREA_POR_PRODUTO" ref="A1:AM25" totalsRowShown="0">
-  <autoFilter ref="A1:AM25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}" name="AREA_POR_PRODUTO" displayName="AREA_POR_PRODUTO" ref="A1:AN25" totalsRowShown="0">
+  <autoFilter ref="A1:AN25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
+  <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{5E4BCC7B-BD3D-4850-9D02-5BDA26FED269}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{CA31088B-0A58-4A64-AE47-76C708B3947A}" name="NORTE" dataDxfId="192"/>
-    <tableColumn id="3" xr3:uid="{49129A23-8E4D-43BD-A688-921DB22B8F95}" name="RR" dataDxfId="191"/>
-    <tableColumn id="4" xr3:uid="{A165E71E-265F-4003-AA0E-8E9F26D12909}" name="RO" dataDxfId="190"/>
-    <tableColumn id="5" xr3:uid="{A386A7C6-C111-4CC7-8C16-FD58B8F0562F}" name="AC" dataDxfId="189"/>
-    <tableColumn id="6" xr3:uid="{9B733D29-A480-4FD0-A166-98AAD1AC2E74}" name="AM" dataDxfId="188"/>
-    <tableColumn id="7" xr3:uid="{F2B3378A-D467-452B-B894-8576A5D41BBE}" name="AP" dataDxfId="187"/>
-    <tableColumn id="8" xr3:uid="{2FE38FD4-49A7-402E-9249-2F1FE7E4E027}" name="PA" dataDxfId="186"/>
-    <tableColumn id="9" xr3:uid="{3F8DA4DF-43C6-4A2E-9793-6FB45F31D88A}" name="TO" dataDxfId="185"/>
-    <tableColumn id="10" xr3:uid="{08FE1121-488E-4A8A-A1D0-3D0D87153D95}" name="NORDESTE" dataDxfId="184"/>
-    <tableColumn id="11" xr3:uid="{DD9EA0BE-AEB8-4904-BE5A-81EC4F42E4C6}" name="MA" dataDxfId="183"/>
-    <tableColumn id="12" xr3:uid="{C65CE50B-DF9F-4EFE-AC1E-19A16468713A}" name="PI" dataDxfId="182"/>
-    <tableColumn id="13" xr3:uid="{5D05969A-E1C7-43A7-B71B-22268FB3E232}" name="CE" dataDxfId="181"/>
-    <tableColumn id="14" xr3:uid="{A97B6897-CFFE-4661-B611-B2D60CCF0ADC}" name="RN" dataDxfId="180"/>
-    <tableColumn id="15" xr3:uid="{BF86C9D2-5807-4F40-9051-7A67068281AA}" name="PB" dataDxfId="179"/>
-    <tableColumn id="16" xr3:uid="{E3A30C52-12FA-4308-ACA5-E511229E5D56}" name="PE" dataDxfId="178"/>
-    <tableColumn id="17" xr3:uid="{986578B0-2D30-422D-AE94-C704D371A9ED}" name="AL" dataDxfId="177"/>
-    <tableColumn id="18" xr3:uid="{61435B55-D3FE-4C3A-812E-CE5D0118E63E}" name="SE" dataDxfId="176"/>
-    <tableColumn id="19" xr3:uid="{534969DF-1823-4F20-A806-97162E402F0E}" name="BA" dataDxfId="175"/>
-    <tableColumn id="20" xr3:uid="{EDE8B247-4C19-4366-8800-9FEBEE13F9EA}" name="CENTRO-OESTE" dataDxfId="174"/>
-    <tableColumn id="21" xr3:uid="{A1667BB6-B217-492E-ACA4-B6E7FA0AF37B}" name="MT" dataDxfId="173"/>
-    <tableColumn id="22" xr3:uid="{54601504-468E-416E-8E4D-408050EFD8F1}" name="MS" dataDxfId="172"/>
-    <tableColumn id="23" xr3:uid="{1CA71861-8B72-40F9-8803-77B24A439D3B}" name="GO" dataDxfId="171"/>
-    <tableColumn id="24" xr3:uid="{D65A4ED9-4AA6-46B6-85F9-FF04865D9CD9}" name="DF" dataDxfId="170"/>
-    <tableColumn id="25" xr3:uid="{84502B60-EABA-40A0-98B8-19B8961F1D37}" name="SUDESTE" dataDxfId="169"/>
-    <tableColumn id="26" xr3:uid="{B60F76A8-80E5-4C5C-9541-1F844E7A3AE1}" name="MG" dataDxfId="168"/>
-    <tableColumn id="27" xr3:uid="{CC4AA6A5-83E1-4E87-A2CC-245EF4F57BFB}" name="ES" dataDxfId="167"/>
-    <tableColumn id="28" xr3:uid="{CA5AB65D-6CEA-4F12-93CA-75E3666C2354}" name="RJ" dataDxfId="166"/>
-    <tableColumn id="29" xr3:uid="{1E391A6D-FDCF-41F4-8790-26376C8AD795}" name="SP" dataDxfId="165"/>
-    <tableColumn id="30" xr3:uid="{04C869B7-96FC-43E9-9CE2-82769EFFDCA0}" name="SUL" dataDxfId="164"/>
-    <tableColumn id="31" xr3:uid="{9DCC0D0C-ACE3-4E6C-966D-A3E9ED01FBB5}" name="PR" dataDxfId="163"/>
-    <tableColumn id="32" xr3:uid="{C1056F8D-2C9F-4314-8424-F2B642B3F545}" name="SC" dataDxfId="162"/>
-    <tableColumn id="33" xr3:uid="{417BD3DD-D799-4503-A0AE-70D3CF2E75F7}" name="RS" dataDxfId="161"/>
-    <tableColumn id="34" xr3:uid="{E9B9638C-63FC-4E3C-9765-611D2BA02CEF}" name="NORTE-NORDESTE" dataDxfId="160"/>
-    <tableColumn id="35" xr3:uid="{BB0E374F-8FC9-4AE4-A4A2-6F762AEF1580}" name="CENTRO-SUL" dataDxfId="159"/>
-    <tableColumn id="36" xr3:uid="{8C7BDB00-4B75-4FF9-8F29-D37982132B90}" name="BRASIL" dataDxfId="158"/>
-    <tableColumn id="37" xr3:uid="{0FF9F8EF-1643-4E16-A1B9-53905A2DD396}" name="ANO" dataDxfId="157"/>
-    <tableColumn id="38" xr3:uid="{A4BC462C-3977-4A40-BE0D-1A25B4C47A2A}" name="MÊS" dataDxfId="156"/>
-    <tableColumn id="39" xr3:uid="{8717C3B1-3F56-4A6D-8272-548CC6EE93AA}" name="SAFRA" dataDxfId="155"/>
+    <tableColumn id="2" xr3:uid="{CA31088B-0A58-4A64-AE47-76C708B3947A}" name="NORTE" dataDxfId="196"/>
+    <tableColumn id="3" xr3:uid="{49129A23-8E4D-43BD-A688-921DB22B8F95}" name="RR" dataDxfId="195"/>
+    <tableColumn id="4" xr3:uid="{A165E71E-265F-4003-AA0E-8E9F26D12909}" name="RO" dataDxfId="194"/>
+    <tableColumn id="5" xr3:uid="{A386A7C6-C111-4CC7-8C16-FD58B8F0562F}" name="AC" dataDxfId="193"/>
+    <tableColumn id="6" xr3:uid="{9B733D29-A480-4FD0-A166-98AAD1AC2E74}" name="AM" dataDxfId="192"/>
+    <tableColumn id="7" xr3:uid="{F2B3378A-D467-452B-B894-8576A5D41BBE}" name="AP" dataDxfId="191"/>
+    <tableColumn id="8" xr3:uid="{2FE38FD4-49A7-402E-9249-2F1FE7E4E027}" name="PA" dataDxfId="190"/>
+    <tableColumn id="9" xr3:uid="{3F8DA4DF-43C6-4A2E-9793-6FB45F31D88A}" name="TO" dataDxfId="189"/>
+    <tableColumn id="10" xr3:uid="{08FE1121-488E-4A8A-A1D0-3D0D87153D95}" name="NORDESTE" dataDxfId="188"/>
+    <tableColumn id="11" xr3:uid="{DD9EA0BE-AEB8-4904-BE5A-81EC4F42E4C6}" name="MA" dataDxfId="187"/>
+    <tableColumn id="12" xr3:uid="{C65CE50B-DF9F-4EFE-AC1E-19A16468713A}" name="PI" dataDxfId="186"/>
+    <tableColumn id="13" xr3:uid="{5D05969A-E1C7-43A7-B71B-22268FB3E232}" name="CE" dataDxfId="185"/>
+    <tableColumn id="14" xr3:uid="{A97B6897-CFFE-4661-B611-B2D60CCF0ADC}" name="RN" dataDxfId="184"/>
+    <tableColumn id="15" xr3:uid="{BF86C9D2-5807-4F40-9051-7A67068281AA}" name="PB" dataDxfId="183"/>
+    <tableColumn id="16" xr3:uid="{E3A30C52-12FA-4308-ACA5-E511229E5D56}" name="PE" dataDxfId="182"/>
+    <tableColumn id="17" xr3:uid="{986578B0-2D30-422D-AE94-C704D371A9ED}" name="AL" dataDxfId="181"/>
+    <tableColumn id="18" xr3:uid="{61435B55-D3FE-4C3A-812E-CE5D0118E63E}" name="SE" dataDxfId="180"/>
+    <tableColumn id="19" xr3:uid="{534969DF-1823-4F20-A806-97162E402F0E}" name="BA" dataDxfId="179"/>
+    <tableColumn id="20" xr3:uid="{EDE8B247-4C19-4366-8800-9FEBEE13F9EA}" name="CENTRO-OESTE" dataDxfId="178"/>
+    <tableColumn id="21" xr3:uid="{A1667BB6-B217-492E-ACA4-B6E7FA0AF37B}" name="MT" dataDxfId="177"/>
+    <tableColumn id="22" xr3:uid="{54601504-468E-416E-8E4D-408050EFD8F1}" name="MS" dataDxfId="176"/>
+    <tableColumn id="23" xr3:uid="{1CA71861-8B72-40F9-8803-77B24A439D3B}" name="GO" dataDxfId="175"/>
+    <tableColumn id="24" xr3:uid="{D65A4ED9-4AA6-46B6-85F9-FF04865D9CD9}" name="DF" dataDxfId="174"/>
+    <tableColumn id="25" xr3:uid="{84502B60-EABA-40A0-98B8-19B8961F1D37}" name="SUDESTE" dataDxfId="173"/>
+    <tableColumn id="26" xr3:uid="{B60F76A8-80E5-4C5C-9541-1F844E7A3AE1}" name="MG" dataDxfId="172"/>
+    <tableColumn id="27" xr3:uid="{CC4AA6A5-83E1-4E87-A2CC-245EF4F57BFB}" name="ES" dataDxfId="171"/>
+    <tableColumn id="28" xr3:uid="{CA5AB65D-6CEA-4F12-93CA-75E3666C2354}" name="RJ" dataDxfId="170"/>
+    <tableColumn id="29" xr3:uid="{1E391A6D-FDCF-41F4-8790-26376C8AD795}" name="SP" dataDxfId="169"/>
+    <tableColumn id="30" xr3:uid="{04C869B7-96FC-43E9-9CE2-82769EFFDCA0}" name="SUL" dataDxfId="168"/>
+    <tableColumn id="31" xr3:uid="{9DCC0D0C-ACE3-4E6C-966D-A3E9ED01FBB5}" name="PR" dataDxfId="167"/>
+    <tableColumn id="32" xr3:uid="{C1056F8D-2C9F-4314-8424-F2B642B3F545}" name="SC" dataDxfId="166"/>
+    <tableColumn id="33" xr3:uid="{417BD3DD-D799-4503-A0AE-70D3CF2E75F7}" name="RS" dataDxfId="165"/>
+    <tableColumn id="34" xr3:uid="{E9B9638C-63FC-4E3C-9765-611D2BA02CEF}" name="NORTE-NORDESTE" dataDxfId="164"/>
+    <tableColumn id="35" xr3:uid="{BB0E374F-8FC9-4AE4-A4A2-6F762AEF1580}" name="CENTRO-SUL" dataDxfId="163"/>
+    <tableColumn id="36" xr3:uid="{8C7BDB00-4B75-4FF9-8F29-D37982132B90}" name="BRASIL" dataDxfId="162"/>
+    <tableColumn id="37" xr3:uid="{0FF9F8EF-1643-4E16-A1B9-53905A2DD396}" name="ANO" dataDxfId="161"/>
+    <tableColumn id="38" xr3:uid="{A4BC462C-3977-4A40-BE0D-1A25B4C47A2A}" name="MÊS" dataDxfId="160"/>
+    <tableColumn id="39" xr3:uid="{8717C3B1-3F56-4A6D-8272-548CC6EE93AA}" name="SAFRA" dataDxfId="159"/>
+    <tableColumn id="40" xr3:uid="{44F23BE6-F9BD-46E4-8A2F-4E8B00F6367C}" name="TIPO" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6AAA68D2-2837-4E56-9205-588FBC25E607}" name="AREA_POR_REGIAO" displayName="AREA_POR_REGIAO" ref="A1:AB36" totalsRowShown="0">
-  <autoFilter ref="A1:AB36" xr:uid="{6AAA68D2-2837-4E56-9205-588FBC25E607}"/>
-  <tableColumns count="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6AAA68D2-2837-4E56-9205-588FBC25E607}" name="AREA_POR_REGIAO" displayName="AREA_POR_REGIAO" ref="A1:AC36" totalsRowShown="0">
+  <autoFilter ref="A1:AC36" xr:uid="{6AAA68D2-2837-4E56-9205-588FBC25E607}"/>
+  <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{9D8E11EB-62E4-4646-82D1-16F281AB841F}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{400D5D9F-14BE-449D-A25E-F770F1684551}" name="ALGODÃO TOTAL" dataDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{1A597964-8010-4331-ABEA-1AEA845AB5F5}" name="ALGODÃO PLUMA" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{B2BFD712-F833-47B4-830F-961CC061703C}" name="ALGODÃO CAROÇO" dataDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{F4D73FDB-EAAE-4D0E-8E22-29A41F3B9E20}" name="AMENDOIM" dataDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{5B9AB598-74CF-401E-9133-20988114821A}" name="ARROZ TOTAL" dataDxfId="150"/>
-    <tableColumn id="7" xr3:uid="{9F25F6FD-273B-47C9-A893-C8D4CAFE7AB6}" name="ARROZ SEQUEIRO" dataDxfId="149"/>
-    <tableColumn id="8" xr3:uid="{C5FEDFF2-6DFD-4C53-869F-F28A5C23DF3B}" name="ARROZ IRRIGADO" dataDxfId="148"/>
-    <tableColumn id="9" xr3:uid="{211D5550-928C-4A68-8D86-E36DF84B0861}" name="FEIJÃO TOTAL" dataDxfId="147"/>
-    <tableColumn id="10" xr3:uid="{9C00CC61-0B0F-43D5-A684-AE913448FB8D}" name="FEIJÃO CORES" dataDxfId="146"/>
-    <tableColumn id="11" xr3:uid="{F00934D7-9B86-45AA-8159-2128826AE03E}" name="FEIJÃO PRETO" dataDxfId="145"/>
-    <tableColumn id="12" xr3:uid="{1CBBEDAF-020E-4EFE-907A-27557665AA02}" name="FEIJÃO CAUPI" dataDxfId="144"/>
-    <tableColumn id="13" xr3:uid="{A8B4A0BB-9E8E-4F8C-9B7B-89F6D688EC32}" name="GERGELIM" dataDxfId="143"/>
-    <tableColumn id="14" xr3:uid="{BD44DF76-DF43-47F8-8A9E-050E54211B27}" name="GIRASSOL" dataDxfId="142"/>
-    <tableColumn id="15" xr3:uid="{E3E75921-B2B5-4327-9628-9461D4B2C97A}" name="MAMONA" dataDxfId="141"/>
-    <tableColumn id="16" xr3:uid="{779BE33D-35AA-4039-A599-BA68B482A978}" name="MILHO" dataDxfId="140"/>
-    <tableColumn id="17" xr3:uid="{AC0C1990-76E8-414D-951C-E60C4646E855}" name="SOJA" dataDxfId="139"/>
-    <tableColumn id="18" xr3:uid="{CC2AD535-2144-4A37-B30C-44803E8E0DC2}" name="SORGO" dataDxfId="138"/>
-    <tableColumn id="19" xr3:uid="{DB09C5E0-C39A-4FE3-A0C4-5F83F16E55BE}" name="AVEIA" dataDxfId="137"/>
-    <tableColumn id="20" xr3:uid="{A5A1A29D-945B-43C5-872F-5D7E2D8C0F4F}" name="CANOLA" dataDxfId="136"/>
-    <tableColumn id="21" xr3:uid="{07F643AF-5A03-40BB-B5E8-C02BD7E21808}" name="CENTEIO" dataDxfId="135"/>
-    <tableColumn id="22" xr3:uid="{6A47C86C-50FC-4E1C-8369-917038B220D3}" name="CEVADA" dataDxfId="134"/>
-    <tableColumn id="23" xr3:uid="{2D22156A-463D-4284-9CD8-69F0E87747E7}" name="TRIGO" dataDxfId="133"/>
-    <tableColumn id="24" xr3:uid="{5ACD3FF0-294A-44A8-8DF0-F447B6863725}" name="TRITICALE" dataDxfId="132"/>
-    <tableColumn id="25" xr3:uid="{E71C1FB1-73E6-456B-8624-C3377581DF94}" name="GERAL" dataDxfId="131"/>
-    <tableColumn id="26" xr3:uid="{8186BB93-C0FE-4341-A195-EA43AAD936F3}" name="ANO" dataDxfId="130"/>
-    <tableColumn id="27" xr3:uid="{87DB167D-5607-4997-951C-88947D3A6327}" name="MÊS" dataDxfId="129"/>
-    <tableColumn id="28" xr3:uid="{C07FA4E5-704A-4BBC-9B48-E235E6FEA795}" name="SAFRA" dataDxfId="128"/>
+    <tableColumn id="2" xr3:uid="{400D5D9F-14BE-449D-A25E-F770F1684551}" name="ALGODÃO TOTAL" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{1A597964-8010-4331-ABEA-1AEA845AB5F5}" name="ALGODÃO PLUMA" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{B2BFD712-F833-47B4-830F-961CC061703C}" name="ALGODÃO CAROÇO" dataDxfId="156"/>
+    <tableColumn id="5" xr3:uid="{F4D73FDB-EAAE-4D0E-8E22-29A41F3B9E20}" name="AMENDOIM" dataDxfId="155"/>
+    <tableColumn id="6" xr3:uid="{5B9AB598-74CF-401E-9133-20988114821A}" name="ARROZ TOTAL" dataDxfId="154"/>
+    <tableColumn id="7" xr3:uid="{9F25F6FD-273B-47C9-A893-C8D4CAFE7AB6}" name="ARROZ SEQUEIRO" dataDxfId="153"/>
+    <tableColumn id="8" xr3:uid="{C5FEDFF2-6DFD-4C53-869F-F28A5C23DF3B}" name="ARROZ IRRIGADO" dataDxfId="152"/>
+    <tableColumn id="9" xr3:uid="{211D5550-928C-4A68-8D86-E36DF84B0861}" name="FEIJÃO TOTAL" dataDxfId="151"/>
+    <tableColumn id="10" xr3:uid="{9C00CC61-0B0F-43D5-A684-AE913448FB8D}" name="FEIJÃO CORES" dataDxfId="150"/>
+    <tableColumn id="11" xr3:uid="{F00934D7-9B86-45AA-8159-2128826AE03E}" name="FEIJÃO PRETO" dataDxfId="149"/>
+    <tableColumn id="12" xr3:uid="{1CBBEDAF-020E-4EFE-907A-27557665AA02}" name="FEIJÃO CAUPI" dataDxfId="148"/>
+    <tableColumn id="13" xr3:uid="{A8B4A0BB-9E8E-4F8C-9B7B-89F6D688EC32}" name="GERGELIM" dataDxfId="147"/>
+    <tableColumn id="14" xr3:uid="{BD44DF76-DF43-47F8-8A9E-050E54211B27}" name="GIRASSOL" dataDxfId="146"/>
+    <tableColumn id="15" xr3:uid="{E3E75921-B2B5-4327-9628-9461D4B2C97A}" name="MAMONA" dataDxfId="145"/>
+    <tableColumn id="16" xr3:uid="{779BE33D-35AA-4039-A599-BA68B482A978}" name="MILHO" dataDxfId="144"/>
+    <tableColumn id="17" xr3:uid="{AC0C1990-76E8-414D-951C-E60C4646E855}" name="SOJA" dataDxfId="143"/>
+    <tableColumn id="18" xr3:uid="{CC2AD535-2144-4A37-B30C-44803E8E0DC2}" name="SORGO" dataDxfId="142"/>
+    <tableColumn id="19" xr3:uid="{DB09C5E0-C39A-4FE3-A0C4-5F83F16E55BE}" name="AVEIA" dataDxfId="141"/>
+    <tableColumn id="20" xr3:uid="{A5A1A29D-945B-43C5-872F-5D7E2D8C0F4F}" name="CANOLA" dataDxfId="140"/>
+    <tableColumn id="21" xr3:uid="{07F643AF-5A03-40BB-B5E8-C02BD7E21808}" name="CENTEIO" dataDxfId="139"/>
+    <tableColumn id="22" xr3:uid="{6A47C86C-50FC-4E1C-8369-917038B220D3}" name="CEVADA" dataDxfId="138"/>
+    <tableColumn id="23" xr3:uid="{2D22156A-463D-4284-9CD8-69F0E87747E7}" name="TRIGO" dataDxfId="137"/>
+    <tableColumn id="24" xr3:uid="{5ACD3FF0-294A-44A8-8DF0-F447B6863725}" name="TRITICALE" dataDxfId="136"/>
+    <tableColumn id="25" xr3:uid="{E71C1FB1-73E6-456B-8624-C3377581DF94}" name="GERAL" dataDxfId="135"/>
+    <tableColumn id="26" xr3:uid="{8186BB93-C0FE-4341-A195-EA43AAD936F3}" name="ANO" dataDxfId="134"/>
+    <tableColumn id="27" xr3:uid="{87DB167D-5607-4997-951C-88947D3A6327}" name="MÊS" dataDxfId="133"/>
+    <tableColumn id="28" xr3:uid="{C07FA4E5-704A-4BBC-9B48-E235E6FEA795}" name="SAFRA" dataDxfId="132"/>
+    <tableColumn id="29" xr3:uid="{B4E655B4-2876-4D39-8C39-CED7CA28A757}" name="TIPO" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6E87F42-FE8A-4067-8EF0-E46E70574C8B}" name="PRODUTIVIDADE_POR_PRODUTO" displayName="PRODUTIVIDADE_POR_PRODUTO" ref="A1:AM25" totalsRowShown="0">
-  <autoFilter ref="A1:AM25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A6E87F42-FE8A-4067-8EF0-E46E70574C8B}" name="PRODUTIVIDADE_POR_PRODUTO" displayName="PRODUTIVIDADE_POR_PRODUTO" ref="A1:AN25" totalsRowShown="0">
+  <autoFilter ref="A1:AN25" xr:uid="{5B7D321A-43AE-4A82-BD55-3D36C41B7E32}"/>
+  <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{8CF1AF50-3446-4E75-8105-3A27A31DC53D}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="125"/>
-    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="124"/>
-    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="123"/>
-    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="122"/>
-    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="121"/>
-    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="120"/>
-    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="119"/>
-    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="118"/>
-    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="117"/>
-    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="116"/>
-    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="115"/>
-    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="114"/>
-    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="113"/>
-    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="112"/>
-    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="111"/>
-    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="110"/>
-    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="109"/>
-    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="108"/>
-    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="107"/>
-    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="106"/>
-    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="105"/>
-    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="104"/>
-    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="103"/>
-    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="102"/>
-    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="101"/>
-    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="100"/>
-    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="99"/>
-    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="98"/>
-    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="97"/>
-    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="96"/>
-    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="95"/>
-    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="94"/>
-    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="93"/>
-    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="92"/>
-    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="91"/>
-    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{B84906ED-0B3E-4BAF-823C-613564EC7F44}" name="NORTE" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{84B9811A-583F-4CE3-B96E-FD8D3F9C0AF7}" name="RR" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{0AFF1D5D-3E87-4339-BBA1-770DC84997E0}" name="RO" dataDxfId="129"/>
+    <tableColumn id="5" xr3:uid="{8E7E000F-2618-4C1D-A0A3-786BAD1CCA1E}" name="AC" dataDxfId="128"/>
+    <tableColumn id="6" xr3:uid="{8FDC185D-309C-44F0-909D-47D36E4E88C7}" name="AM" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{FCFBA294-1B56-4D43-81BD-8397D063FB54}" name="AP" dataDxfId="126"/>
+    <tableColumn id="8" xr3:uid="{A4D89CF5-1E5F-4A95-9E6F-6AF87D6DC899}" name="PA" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{CBEB4E66-65D5-43C3-A560-E78883927AF4}" name="TO" dataDxfId="124"/>
+    <tableColumn id="10" xr3:uid="{E7D25C84-64C7-44D2-85A6-1289EF929C61}" name="NORDESTE" dataDxfId="123"/>
+    <tableColumn id="11" xr3:uid="{3A9FA498-3724-4EB1-92DC-966AAB9D214D}" name="MA" dataDxfId="122"/>
+    <tableColumn id="12" xr3:uid="{217BE2AA-49BC-4EFB-A2E9-A68DAFEE98F1}" name="PI" dataDxfId="121"/>
+    <tableColumn id="13" xr3:uid="{2A2F8CD6-E44E-48F7-95FF-898DA8413AFD}" name="CE" dataDxfId="120"/>
+    <tableColumn id="14" xr3:uid="{A6E9090C-1AB9-4D6E-9F99-ABDA730D9CA6}" name="RN" dataDxfId="119"/>
+    <tableColumn id="15" xr3:uid="{C74DAA05-C155-4F4D-B631-EB31FBB3665F}" name="PB" dataDxfId="118"/>
+    <tableColumn id="16" xr3:uid="{E5A10D15-FEE8-4661-ADBA-FB28CEA9267C}" name="PE" dataDxfId="117"/>
+    <tableColumn id="17" xr3:uid="{D1DA04F7-F9F0-4017-AE33-C5C1E7CE5AC0}" name="AL" dataDxfId="116"/>
+    <tableColumn id="18" xr3:uid="{DD2B9F5D-C570-466E-82CC-C54D2042ADFD}" name="SE" dataDxfId="115"/>
+    <tableColumn id="19" xr3:uid="{A2536CAA-3E99-4275-8AFB-0F230AD1FE08}" name="BA" dataDxfId="114"/>
+    <tableColumn id="20" xr3:uid="{C9DE622E-9653-49C4-97A9-6F44C0598F06}" name="CENTRO-OESTE" dataDxfId="113"/>
+    <tableColumn id="21" xr3:uid="{625EA772-B512-443B-A734-AF5CE77AB668}" name="MT" dataDxfId="112"/>
+    <tableColumn id="22" xr3:uid="{71A57575-7815-481F-AAAC-8C1EE9703912}" name="MS" dataDxfId="111"/>
+    <tableColumn id="23" xr3:uid="{F0365580-4820-46C6-A7D7-BD7C897237CB}" name="GO" dataDxfId="110"/>
+    <tableColumn id="24" xr3:uid="{A5D6C791-8D94-4B52-8C0C-39F7AD4AC4E1}" name="DF" dataDxfId="109"/>
+    <tableColumn id="25" xr3:uid="{3C464D88-F9B1-4C7A-8784-1840561093C3}" name="SUDESTE" dataDxfId="108"/>
+    <tableColumn id="26" xr3:uid="{1184085B-389F-4DFA-BAAA-79A73F5D58E9}" name="MG" dataDxfId="107"/>
+    <tableColumn id="27" xr3:uid="{1FD7AAC9-8B22-4599-8C41-97B306E682A8}" name="ES" dataDxfId="106"/>
+    <tableColumn id="28" xr3:uid="{3789E530-8644-46B9-A1D9-538F173953B6}" name="RJ" dataDxfId="105"/>
+    <tableColumn id="29" xr3:uid="{4B510379-3A08-42EB-8F76-653D7A9A0F0C}" name="SP" dataDxfId="104"/>
+    <tableColumn id="30" xr3:uid="{B7137113-AFD6-4F75-AE3E-0C0A27D770EB}" name="SUL" dataDxfId="103"/>
+    <tableColumn id="31" xr3:uid="{725B070C-B20E-4909-860C-25B32C284E06}" name="PR" dataDxfId="102"/>
+    <tableColumn id="32" xr3:uid="{4407D65F-AE79-48AC-9A84-33DCE4A2ADA4}" name="SC" dataDxfId="101"/>
+    <tableColumn id="33" xr3:uid="{88C455AC-C842-489F-84B2-E60D576F9F16}" name="RS" dataDxfId="100"/>
+    <tableColumn id="34" xr3:uid="{F04DD72A-4B16-4880-860B-5C4A2F256C93}" name="NORTE-NORDESTE" dataDxfId="99"/>
+    <tableColumn id="35" xr3:uid="{83D2B4A6-D70A-4652-89BB-1ED9B337F34A}" name="CENTRO-SUL" dataDxfId="98"/>
+    <tableColumn id="36" xr3:uid="{E90095A4-CB96-450E-A159-B808E8913751}" name="BRASIL" dataDxfId="97"/>
+    <tableColumn id="37" xr3:uid="{5796B11A-3AF2-4B43-92FF-178971C3DBD9}" name="ANO" dataDxfId="96"/>
+    <tableColumn id="38" xr3:uid="{5B4B4C2C-6AED-479F-B62E-92551DACC89D}" name="MÊS" dataDxfId="95"/>
+    <tableColumn id="39" xr3:uid="{453C9B87-B335-49FF-BF33-6444C74EE93B}" name="SAFRA" dataDxfId="94"/>
+    <tableColumn id="40" xr3:uid="{2714208A-1A54-49BE-818E-BC69C2F93175}" name="TIPO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}" name="PRODUTIVIDADE_POR_REGIAO" displayName="PRODUTIVIDADE_POR_REGIAO" ref="A1:AB36" totalsRowShown="0">
-  <autoFilter ref="A1:AB36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
-  <tableColumns count="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}" name="PRODUTIVIDADE_POR_REGIAO" displayName="PRODUTIVIDADE_POR_REGIAO" ref="A1:AC36" totalsRowShown="0">
+  <autoFilter ref="A1:AC36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
+  <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{DAF3B878-FB08-46CD-ACA1-18181EFBFBAD}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{696769AD-331A-446B-8AC3-B7C2D6DFB4E8}" name="ALGODÃO TOTAL" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{5E665A64-E5CA-4198-9ED1-223E0FFF8B1A}" name="ALGODÃO PLUMA" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{57ADDDDD-9A37-44E9-983C-5B9F0D61AF11}" name="ALGODÃO CAROÇO" dataDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{BD6D0D9E-BA32-4F0C-BAA5-432806AD0AA9}" name="AMENDOIM" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{C681D5C9-AA19-42EE-BA4D-84A974B167AB}" name="ARROZ TOTAL" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{21C89C02-6582-4EA1-885A-BE6F358EFB65}" name="ARROZ SEQUEIRO" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{501ED1B5-AC3F-4814-A140-66E033D4A6D8}" name="ARROZ IRRIGADO" dataDxfId="83"/>
-    <tableColumn id="9" xr3:uid="{04AD2B17-EAE9-468E-9CE2-F9622EDD8FAB}" name="FEIJÃO TOTAL" dataDxfId="82"/>
-    <tableColumn id="10" xr3:uid="{42CBB38A-7B8E-4D57-921D-C225BD11BA37}" name="FEIJÃO CORES" dataDxfId="81"/>
-    <tableColumn id="11" xr3:uid="{2D91C5A5-E4B0-489B-803D-F2729F4C4F74}" name="FEIJÃO PRETO" dataDxfId="80"/>
-    <tableColumn id="12" xr3:uid="{99C1F29D-95F7-4EEA-8358-7E1C3C68D9BD}" name="FEIJÃO CAUPI" dataDxfId="79"/>
-    <tableColumn id="13" xr3:uid="{B56D35BC-0CE8-4B2C-AA42-0F259574BA42}" name="GERGELIM" dataDxfId="78"/>
-    <tableColumn id="14" xr3:uid="{DCA5F91F-E4C7-409B-8D7D-D7CB01BD5BD4}" name="GIRASSOL" dataDxfId="77"/>
-    <tableColumn id="15" xr3:uid="{C4FEE6B7-7EF6-456E-B8DE-D28E6D59FC75}" name="MAMONA" dataDxfId="76"/>
-    <tableColumn id="16" xr3:uid="{1355C0D1-26AC-4CDD-97CF-BBF69AC27943}" name="MILHO" dataDxfId="75"/>
-    <tableColumn id="17" xr3:uid="{F87E309F-FB19-4F9B-AF8A-791408964512}" name="SOJA" dataDxfId="74"/>
-    <tableColumn id="18" xr3:uid="{C3B3364B-EC9C-4949-8747-10B77423825C}" name="SORGO" dataDxfId="73"/>
-    <tableColumn id="19" xr3:uid="{24AFF494-F277-42E7-BB5C-7D4DD4610D0A}" name="AVEIA" dataDxfId="72"/>
-    <tableColumn id="20" xr3:uid="{AA50ABAF-470B-4E78-B762-C184C2002B38}" name="CANOLA" dataDxfId="71"/>
-    <tableColumn id="21" xr3:uid="{E41B718D-8512-4FBA-94E7-68D66488A5A3}" name="CENTEIO" dataDxfId="70"/>
-    <tableColumn id="22" xr3:uid="{5FD3C437-7E82-475D-BB2A-21A8CCFB39A8}" name="CEVADA" dataDxfId="69"/>
-    <tableColumn id="23" xr3:uid="{521DED51-CA6F-48F2-89ED-A38C0B449C5F}" name="TRIGO" dataDxfId="68"/>
-    <tableColumn id="24" xr3:uid="{C71EED0F-A05C-4902-876D-30647F78380D}" name="TRITICALE" dataDxfId="67"/>
-    <tableColumn id="25" xr3:uid="{43F11742-31FE-47CA-9206-DE9A85BDFA19}" name="GERAL" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{696769AD-331A-446B-8AC3-B7C2D6DFB4E8}" name="ALGODÃO TOTAL" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{5E665A64-E5CA-4198-9ED1-223E0FFF8B1A}" name="ALGODÃO PLUMA" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{57ADDDDD-9A37-44E9-983C-5B9F0D61AF11}" name="ALGODÃO CAROÇO" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{BD6D0D9E-BA32-4F0C-BAA5-432806AD0AA9}" name="AMENDOIM" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{C681D5C9-AA19-42EE-BA4D-84A974B167AB}" name="ARROZ TOTAL" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{21C89C02-6582-4EA1-885A-BE6F358EFB65}" name="ARROZ SEQUEIRO" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{501ED1B5-AC3F-4814-A140-66E033D4A6D8}" name="ARROZ IRRIGADO" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{04AD2B17-EAE9-468E-9CE2-F9622EDD8FAB}" name="FEIJÃO TOTAL" dataDxfId="86"/>
+    <tableColumn id="10" xr3:uid="{42CBB38A-7B8E-4D57-921D-C225BD11BA37}" name="FEIJÃO CORES" dataDxfId="85"/>
+    <tableColumn id="11" xr3:uid="{2D91C5A5-E4B0-489B-803D-F2729F4C4F74}" name="FEIJÃO PRETO" dataDxfId="84"/>
+    <tableColumn id="12" xr3:uid="{99C1F29D-95F7-4EEA-8358-7E1C3C68D9BD}" name="FEIJÃO CAUPI" dataDxfId="83"/>
+    <tableColumn id="13" xr3:uid="{B56D35BC-0CE8-4B2C-AA42-0F259574BA42}" name="GERGELIM" dataDxfId="82"/>
+    <tableColumn id="14" xr3:uid="{DCA5F91F-E4C7-409B-8D7D-D7CB01BD5BD4}" name="GIRASSOL" dataDxfId="81"/>
+    <tableColumn id="15" xr3:uid="{C4FEE6B7-7EF6-456E-B8DE-D28E6D59FC75}" name="MAMONA" dataDxfId="80"/>
+    <tableColumn id="16" xr3:uid="{1355C0D1-26AC-4CDD-97CF-BBF69AC27943}" name="MILHO" dataDxfId="79"/>
+    <tableColumn id="17" xr3:uid="{F87E309F-FB19-4F9B-AF8A-791408964512}" name="SOJA" dataDxfId="78"/>
+    <tableColumn id="18" xr3:uid="{C3B3364B-EC9C-4949-8747-10B77423825C}" name="SORGO" dataDxfId="77"/>
+    <tableColumn id="19" xr3:uid="{24AFF494-F277-42E7-BB5C-7D4DD4610D0A}" name="AVEIA" dataDxfId="76"/>
+    <tableColumn id="20" xr3:uid="{AA50ABAF-470B-4E78-B762-C184C2002B38}" name="CANOLA" dataDxfId="75"/>
+    <tableColumn id="21" xr3:uid="{E41B718D-8512-4FBA-94E7-68D66488A5A3}" name="CENTEIO" dataDxfId="74"/>
+    <tableColumn id="22" xr3:uid="{5FD3C437-7E82-475D-BB2A-21A8CCFB39A8}" name="CEVADA" dataDxfId="73"/>
+    <tableColumn id="23" xr3:uid="{521DED51-CA6F-48F2-89ED-A38C0B449C5F}" name="TRIGO" dataDxfId="72"/>
+    <tableColumn id="24" xr3:uid="{C71EED0F-A05C-4902-876D-30647F78380D}" name="TRITICALE" dataDxfId="71"/>
+    <tableColumn id="25" xr3:uid="{43F11742-31FE-47CA-9206-DE9A85BDFA19}" name="GERAL" dataDxfId="70"/>
     <tableColumn id="26" xr3:uid="{C21B5348-2002-46F8-AF76-43C13BCC151D}" name="ANO"/>
-    <tableColumn id="27" xr3:uid="{D891F035-96D6-480F-919B-B57924EE851E}" name="MÊS" dataDxfId="65"/>
-    <tableColumn id="28" xr3:uid="{0232FBA8-C0E4-432C-A673-68FECC15080F}" name="SAFRA" dataDxfId="64"/>
+    <tableColumn id="27" xr3:uid="{D891F035-96D6-480F-919B-B57924EE851E}" name="MÊS" dataDxfId="69"/>
+    <tableColumn id="28" xr3:uid="{0232FBA8-C0E4-432C-A673-68FECC15080F}" name="SAFRA" dataDxfId="68"/>
+    <tableColumn id="29" xr3:uid="{28D78BD1-87C0-404F-8DAB-3E6DCD790A67}" name="TIPO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}" name="PRODUCAO_POR_PRODUTO" displayName="PRODUCAO_POR_PRODUTO" ref="A1:AM25" totalsRowShown="0">
-  <autoFilter ref="A1:AM25" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}" name="PRODUCAO_POR_PRODUTO" displayName="PRODUCAO_POR_PRODUTO" ref="A1:AN25" totalsRowShown="0">
+  <autoFilter ref="A1:AN25" xr:uid="{F205EC7A-49EF-4699-9240-6A619C4E0678}"/>
+  <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{6051C5E2-E2B7-4BEB-BC76-2DCAA50A7C15}" name="PRODUTO"/>
-    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="52"/>
-    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="51"/>
-    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="50"/>
-    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="49"/>
-    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="48"/>
-    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="47"/>
-    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="46"/>
-    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="45"/>
-    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="44"/>
-    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="43"/>
-    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="42"/>
-    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="41"/>
-    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="40"/>
-    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="39"/>
-    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="38"/>
-    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="37"/>
-    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="36"/>
-    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="35"/>
-    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="34"/>
-    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="33"/>
-    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="32"/>
-    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="31"/>
-    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="30"/>
-    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="29"/>
-    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="28"/>
-    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="27"/>
-    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{B8D0D550-3F4A-455D-B730-DC7BB52A9B2A}" name="NORTE" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{F0C3B647-0AA7-4BDE-9C13-1E481DDA789C}" name="RR" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{2118BB87-FCC8-403D-8FCA-D68B9ED42B8C}" name="RO" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{3CA4EDC5-768A-430C-8DF0-0D22D3452853}" name="AC" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{7362E812-6294-4692-A499-A02354A455C2}" name="AM" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{482DE189-3576-4B8E-BF1A-9C58B5F5C6ED}" name="AP" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{0E0FA7BD-E6EA-426B-B8B1-9665A67EE819}" name="PA" dataDxfId="61"/>
+    <tableColumn id="9" xr3:uid="{9ABF8262-0C59-4BAA-8D66-6D70743CECED}" name="TO" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{96D8ACAF-FFFE-4005-ADC1-94AA97CD6038}" name="NORDESTE" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{1FABF4C2-AC99-4575-B4A2-682FB02C27AB}" name="MA" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{6E7000A1-CF81-4A5C-AF79-B5A606493E58}" name="PI" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{5804C6F2-0132-4A60-8701-6454E76B39E1}" name="CE" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{FAC246D4-9925-4737-BA6E-C12890CC3492}" name="RN" dataDxfId="55"/>
+    <tableColumn id="15" xr3:uid="{70365A79-11D8-4822-868C-B390282D31AA}" name="PB" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{C5EA46D4-2A74-4A1B-8628-EDE27732EBC1}" name="PE" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{3AB16384-A9C1-4EAE-B1D3-B6980668DDFB}" name="AL" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{5550B480-640D-47F3-98E2-47360C39B350}" name="SE" dataDxfId="51"/>
+    <tableColumn id="19" xr3:uid="{AC7410A2-BEC3-4F36-9DE3-007ABEDAFE77}" name="BA" dataDxfId="50"/>
+    <tableColumn id="20" xr3:uid="{EF9CC834-4DE2-4F12-A01F-E188C35BB745}" name="CENTRO-OESTE" dataDxfId="49"/>
+    <tableColumn id="21" xr3:uid="{43361983-B660-4F10-8172-158B7FE088A3}" name="MT" dataDxfId="48"/>
+    <tableColumn id="22" xr3:uid="{1D87111A-4709-4B48-BC75-F06DA78D87CB}" name="MS" dataDxfId="47"/>
+    <tableColumn id="23" xr3:uid="{8C8B08DD-2483-4E25-AB6C-69DC01B3EB3D}" name="GO" dataDxfId="46"/>
+    <tableColumn id="24" xr3:uid="{9D3A4E55-E1CC-4509-9BBA-1BA1B5720931}" name="DF" dataDxfId="45"/>
+    <tableColumn id="25" xr3:uid="{64CEA2A0-9627-43CF-9192-24F44872CC96}" name="SUDESTE" dataDxfId="44"/>
+    <tableColumn id="26" xr3:uid="{4FBE3EC3-154E-4DF3-ABB6-B6DEFFC26271}" name="MG" dataDxfId="43"/>
+    <tableColumn id="27" xr3:uid="{B6B47D99-4133-4D01-BF64-2BBBE6D3BE49}" name="ES" dataDxfId="42"/>
+    <tableColumn id="28" xr3:uid="{7CC112A7-D0E8-4317-B401-EC4CD011155C}" name="RJ" dataDxfId="41"/>
+    <tableColumn id="29" xr3:uid="{14E6FF96-46F0-467D-A5A3-F1C831072AA9}" name="SP" dataDxfId="40"/>
+    <tableColumn id="30" xr3:uid="{932BDB91-3454-40CD-B097-52A8AA0A2F81}" name="SUL" dataDxfId="39"/>
+    <tableColumn id="31" xr3:uid="{AA858ED8-15B1-4985-9F57-E0EE2783C677}" name="PR" dataDxfId="38"/>
+    <tableColumn id="32" xr3:uid="{D302D227-008B-444D-87CF-C19499331330}" name="SC" dataDxfId="37"/>
+    <tableColumn id="33" xr3:uid="{65AB5642-25AB-4920-8029-D56BC42AB123}" name="RS" dataDxfId="36"/>
+    <tableColumn id="34" xr3:uid="{7666B84C-5946-494A-83CA-2B24D2CF0DC8}" name="NORTE-NORDESTE" dataDxfId="35"/>
+    <tableColumn id="35" xr3:uid="{633B8894-AE4A-45AC-B1C9-B4EAA702D9F9}" name="CENTRO-SUL" dataDxfId="34"/>
+    <tableColumn id="36" xr3:uid="{6BB08E62-BEF0-4192-83F6-2E12E9E586B8}" name="BRASIL" dataDxfId="33"/>
+    <tableColumn id="37" xr3:uid="{ECC44396-0C86-4DF0-B859-53097AD13988}" name="ANO" dataDxfId="32"/>
+    <tableColumn id="38" xr3:uid="{57AEF2DA-BFBE-4B5B-ABC0-477C4D3CA382}" name="MÊS" dataDxfId="31"/>
+    <tableColumn id="39" xr3:uid="{4AF1745A-E1C0-4A75-AFC1-E75F141DCCAA}" name="SAFRA" dataDxfId="30"/>
+    <tableColumn id="40" xr3:uid="{F8F8992A-CE0C-4507-8BC7-856F34FF00CB}" name="TIPO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D31E3FB7-06A9-4F00-8000-681192EE3207}" name="PRODUCAO_POR_REGIAO" displayName="PRODUCAO_POR_REGIAO" ref="A1:AB36" totalsRowShown="0">
-  <autoFilter ref="A1:AB36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
-  <tableColumns count="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D31E3FB7-06A9-4F00-8000-681192EE3207}" name="PRODUCAO_POR_REGIAO" displayName="PRODUCAO_POR_REGIAO" ref="A1:AC36" totalsRowShown="0">
+  <autoFilter ref="A1:AC36" xr:uid="{51B9CBF4-A819-4208-A9FE-4497BC6B95BA}"/>
+  <tableColumns count="29">
     <tableColumn id="1" xr3:uid="{97EFA303-A9FC-46C0-A365-D8BFD6B07F4E}" name="REGIÃO"/>
-    <tableColumn id="2" xr3:uid="{CD1BE27C-2122-4E57-BF75-B4E0FA407680}" name="ALGODÃO TOTAL" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{6AAC4787-45BB-49C3-925E-EB86773D0EE3}" name="ALGODÃO PLUMA" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{A709C33E-0EFD-439D-AFA6-DCBE5DFECC09}" name="ALGODÃO CAROÇO" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{36919ACC-6DBD-4BA6-B171-C06771CAA181}" name="AMENDOIM" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{A9E1ECF8-9280-4528-BB2D-F3444CC4E573}" name="ARROZ TOTAL" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{E24CCEF1-19C6-4E7E-8519-F2CBD6FFBD2C}" name="ARROZ SEQUEIRO" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{27262FD4-F510-4739-AE4D-503E89394540}" name="ARROZ IRRIGADO" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{07A828EE-65C2-453C-98A5-132A6F8EEB49}" name="FEIJÃO TOTAL" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{77436711-59D7-4D39-A13D-93314192FF57}" name="FEIJÃO CORES" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{C39CBBE1-C887-4FAA-B20D-BEF14F189268}" name="FEIJÃO PRETO" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{793D8F4C-ED63-45E7-81EC-8827A45470EF}" name="FEIJÃO CAUPI" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{59CC00D7-C96D-4832-9F17-68AA9395C332}" name="GERGELIM" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{6F397307-9E9A-4B49-89A4-0D105DC65A10}" name="GIRASSOL" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{76D545D2-CB23-48DD-AB8A-DAF6093C755D}" name="MAMONA" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{72E88D52-C6D2-4CF2-8498-8A5F1E83E6C7}" name="MILHO" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{4972AB7E-DAFC-42EA-8460-6CE3DFB48C04}" name="SOJA" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{C27C81AD-E84C-4DB4-9290-8E1075D91C93}" name="SORGO" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{0A447A82-E343-410A-8854-08B23C052F47}" name="AVEIA" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{F5ED3C8B-B7CB-452E-96A2-FCCEB899C54E}" name="CANOLA" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{17829594-1EEC-4783-9488-1309944A44E5}" name="CENTEIO" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CD1BE27C-2122-4E57-BF75-B4E0FA407680}" name="ALGODÃO TOTAL" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{6AAC4787-45BB-49C3-925E-EB86773D0EE3}" name="ALGODÃO PLUMA" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{A709C33E-0EFD-439D-AFA6-DCBE5DFECC09}" name="ALGODÃO CAROÇO" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{36919ACC-6DBD-4BA6-B171-C06771CAA181}" name="AMENDOIM" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{A9E1ECF8-9280-4528-BB2D-F3444CC4E573}" name="ARROZ TOTAL" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{E24CCEF1-19C6-4E7E-8519-F2CBD6FFBD2C}" name="ARROZ SEQUEIRO" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{27262FD4-F510-4739-AE4D-503E89394540}" name="ARROZ IRRIGADO" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{07A828EE-65C2-453C-98A5-132A6F8EEB49}" name="FEIJÃO TOTAL" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{77436711-59D7-4D39-A13D-93314192FF57}" name="FEIJÃO CORES" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{C39CBBE1-C887-4FAA-B20D-BEF14F189268}" name="FEIJÃO PRETO" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{793D8F4C-ED63-45E7-81EC-8827A45470EF}" name="FEIJÃO CAUPI" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{59CC00D7-C96D-4832-9F17-68AA9395C332}" name="GERGELIM" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{6F397307-9E9A-4B49-89A4-0D105DC65A10}" name="GIRASSOL" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{76D545D2-CB23-48DD-AB8A-DAF6093C755D}" name="MAMONA" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{72E88D52-C6D2-4CF2-8498-8A5F1E83E6C7}" name="MILHO" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{4972AB7E-DAFC-42EA-8460-6CE3DFB48C04}" name="SOJA" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{C27C81AD-E84C-4DB4-9290-8E1075D91C93}" name="SORGO" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{0A447A82-E343-410A-8854-08B23C052F47}" name="AVEIA" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{F5ED3C8B-B7CB-452E-96A2-FCCEB899C54E}" name="CANOLA" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{17829594-1EEC-4783-9488-1309944A44E5}" name="CENTEIO" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{49B2C1E3-0396-4037-BB4B-32C18FDB6CC7}" name="CEVADA" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{C10C34AB-D106-4FB2-B097-C90EF653E9E5}" name="TRIGO" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{80045204-E6E2-42D6-9449-CCD3B9641988}" name="TRITICALE" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{0FB9C96B-75F4-4026-A109-A799A828C96B}" name="GERAL" dataDxfId="6"/>
     <tableColumn id="26" xr3:uid="{FA0650E0-02EE-433A-927B-8DCFAD627C43}" name="ANO"/>
-    <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="25"/>
-    <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="24"/>
+    <tableColumn id="27" xr3:uid="{94C00EC6-AB2D-4D90-B787-2C1FF57B5832}" name="MÊS" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{57AFB38B-E07E-457A-9571-EB539326E109}" name="SAFRA" dataDxfId="4"/>
+    <tableColumn id="29" xr3:uid="{DC5A90C4-4F57-40B2-A580-338A1714C27B}" name="TIPO"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1399,11 +1429,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AN26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ34" sqref="AJ34"/>
+      <selection pane="topRight" activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1455,7 @@
     <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,8 +1573,11 @@
       <c r="AM1" t="s">
         <v>62</v>
       </c>
+      <c r="AN1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1662,8 +1695,11 @@
       <c r="AM2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN2" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1781,8 +1817,11 @@
       <c r="AM3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN3" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1900,8 +1939,11 @@
       <c r="AM4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN4" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2019,8 +2061,11 @@
       <c r="AM5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN5" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2138,8 +2183,11 @@
       <c r="AM6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN6" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2257,8 +2305,11 @@
       <c r="AM7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN7" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2376,8 +2427,11 @@
       <c r="AM8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN8" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -2495,8 +2549,11 @@
       <c r="AM9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN9" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2614,8 +2671,11 @@
       <c r="AM10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN10" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2733,8 +2793,11 @@
       <c r="AM11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN11" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2852,8 +2915,11 @@
       <c r="AM12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN12" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -2971,8 +3037,11 @@
       <c r="AM13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN13" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3090,8 +3159,11 @@
       <c r="AM14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN14" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3209,8 +3281,11 @@
       <c r="AM15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN15" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -3328,8 +3403,11 @@
       <c r="AM16" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN16" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -3447,8 +3525,11 @@
       <c r="AM17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN17" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -3566,8 +3647,11 @@
       <c r="AM18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN18" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -3685,8 +3769,11 @@
       <c r="AM19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN19" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -3804,8 +3891,11 @@
       <c r="AM20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN20" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -3923,8 +4013,11 @@
       <c r="AM21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN21" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -4042,8 +4135,11 @@
       <c r="AM22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN22" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -4161,8 +4257,11 @@
       <c r="AM23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN23" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -4280,8 +4379,11 @@
       <c r="AM24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN24" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -4399,8 +4501,11 @@
       <c r="AM25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN25" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="AK26" s="2"/>
       <c r="AL26" s="2"/>
       <c r="AM26" s="2"/>
@@ -4416,10 +4521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B751A56-DEA9-4576-9751-6411F3002DDE}">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="AC2" sqref="AC2:AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4449,7 +4554,7 @@
     <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -4534,8 +4639,11 @@
       <c r="AB1" t="s">
         <v>62</v>
       </c>
+      <c r="AC1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4620,8 +4728,11 @@
       <c r="AB2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC2" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4706,8 +4817,11 @@
       <c r="AB3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC3" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4792,8 +4906,11 @@
       <c r="AB4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC4" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4878,8 +4995,11 @@
       <c r="AB5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC5" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4964,8 +5084,11 @@
       <c r="AB6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC6" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -5050,8 +5173,11 @@
       <c r="AB7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC7" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5136,8 +5262,11 @@
       <c r="AB8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC8" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5222,8 +5351,11 @@
       <c r="AB9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC9" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5308,8 +5440,11 @@
       <c r="AB10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC10" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5394,8 +5529,11 @@
       <c r="AB11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC11" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5480,8 +5618,11 @@
       <c r="AB12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC12" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5566,8 +5707,11 @@
       <c r="AB13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC13" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5652,8 +5796,11 @@
       <c r="AB14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC14" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5738,8 +5885,11 @@
       <c r="AB15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC15" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5824,8 +5974,11 @@
       <c r="AB16" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC16" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5910,8 +6063,11 @@
       <c r="AB17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC17" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -5996,8 +6152,11 @@
       <c r="AB18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC18" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -6082,8 +6241,11 @@
       <c r="AB19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC19" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -6168,8 +6330,11 @@
       <c r="AB20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC20" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -6254,8 +6419,11 @@
       <c r="AB21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC21" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -6340,8 +6508,11 @@
       <c r="AB22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC22" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -6426,8 +6597,11 @@
       <c r="AB23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC23" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -6512,8 +6686,11 @@
       <c r="AB24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC24" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -6598,8 +6775,11 @@
       <c r="AB25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC25" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -6684,8 +6864,11 @@
       <c r="AB26" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC26" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -6770,8 +6953,11 @@
       <c r="AB27" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC27" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -6856,8 +7042,11 @@
       <c r="AB28" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC28" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -6942,8 +7131,11 @@
       <c r="AB29" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC29" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -7028,8 +7220,11 @@
       <c r="AB30" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC30" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -7114,8 +7309,11 @@
       <c r="AB31" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC31" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -7200,8 +7398,11 @@
       <c r="AB32" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC32" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -7286,8 +7487,11 @@
       <c r="AB33" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC33" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -7372,8 +7576,11 @@
       <c r="AB34" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC34" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -7458,8 +7665,11 @@
       <c r="AB35" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC35" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -7543,6 +7753,9 @@
       </c>
       <c r="AB36" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AC36" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -7556,11 +7769,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADAAA7-57A0-4A48-85BB-92E93E4D0781}">
-  <dimension ref="A1:AM26"/>
+  <dimension ref="A1:AN26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:AJ25"/>
+      <selection pane="topRight" activeCell="AN2" sqref="AN2:AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7579,9 +7792,10 @@
     <col min="35" max="35" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7699,8 +7913,11 @@
       <c r="AM1" t="s">
         <v>62</v>
       </c>
+      <c r="AN1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -7818,8 +8035,11 @@
       <c r="AM2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN2" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -7937,8 +8157,11 @@
       <c r="AM3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN3" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -8056,8 +8279,11 @@
       <c r="AM4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN4" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -8175,8 +8401,11 @@
       <c r="AM5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN5" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -8294,8 +8523,11 @@
       <c r="AM6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN6" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -8413,8 +8645,11 @@
       <c r="AM7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN7" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -8532,8 +8767,11 @@
       <c r="AM8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN8" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -8651,8 +8889,11 @@
       <c r="AM9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN9" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -8770,8 +9011,11 @@
       <c r="AM10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN10" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -8889,8 +9133,11 @@
       <c r="AM11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN11" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -9008,8 +9255,11 @@
       <c r="AM12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN12" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -9127,8 +9377,11 @@
       <c r="AM13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN13" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -9246,8 +9499,11 @@
       <c r="AM14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN14" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -9365,8 +9621,11 @@
       <c r="AM15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN15" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -9484,8 +9743,11 @@
       <c r="AM16" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN16" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -9603,8 +9865,11 @@
       <c r="AM17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN17" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -9722,8 +9987,11 @@
       <c r="AM18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN18" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -9841,8 +10109,11 @@
       <c r="AM19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN19" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -9960,8 +10231,11 @@
       <c r="AM20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN20" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -10079,8 +10353,11 @@
       <c r="AM21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN21" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -10198,8 +10475,11 @@
       <c r="AM22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN22" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -10317,8 +10597,11 @@
       <c r="AM23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN23" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -10436,8 +10719,11 @@
       <c r="AM24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN24" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -10555,8 +10841,11 @@
       <c r="AM25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN25" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -10608,8 +10897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BCD6B43-6B79-4F6C-BEBB-EEE94FDB59C5}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AC36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10635,6 +10924,7 @@
     <col min="24" max="24" width="11.7109375" customWidth="1"/>
     <col min="25" max="25" width="10.85546875" customWidth="1"/>
     <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19.140625" customWidth="1"/>
@@ -10643,7 +10933,7 @@
     <col min="38" max="38" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -10728,8 +11018,11 @@
       <c r="AB1" t="s">
         <v>62</v>
       </c>
+      <c r="AC1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -10814,8 +11107,11 @@
       <c r="AB2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC2" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -10900,8 +11196,11 @@
       <c r="AB3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC3" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -10986,8 +11285,11 @@
       <c r="AB4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC4" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -11072,8 +11374,11 @@
       <c r="AB5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC5" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -11158,8 +11463,11 @@
       <c r="AB6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC6" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -11244,8 +11552,11 @@
       <c r="AB7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC7" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -11330,8 +11641,11 @@
       <c r="AB8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC8" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -11416,8 +11730,11 @@
       <c r="AB9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC9" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -11502,8 +11819,11 @@
       <c r="AB10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC10" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -11588,8 +11908,11 @@
       <c r="AB11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC11" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -11674,8 +11997,11 @@
       <c r="AB12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC12" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -11760,8 +12086,11 @@
       <c r="AB13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC13" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -11846,8 +12175,11 @@
       <c r="AB14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC14" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -11932,8 +12264,11 @@
       <c r="AB15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC15" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -12017,6 +12352,9 @@
       </c>
       <c r="AB16" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -12104,6 +12442,9 @@
       <c r="AB17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -12190,6 +12531,9 @@
       <c r="AB18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -12276,6 +12620,9 @@
       <c r="AB19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC19" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -12362,6 +12709,9 @@
       <c r="AB20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC20" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -12448,6 +12798,9 @@
       <c r="AB21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC21" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -12534,6 +12887,9 @@
       <c r="AB22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC22" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -12620,6 +12976,9 @@
       <c r="AB23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC23" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -12706,6 +13065,9 @@
       <c r="AB24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC24" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -12792,6 +13154,9 @@
       <c r="AB25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC25" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -12878,7 +13243,9 @@
       <c r="AB26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AC26" s="1"/>
+      <c r="AC26" t="s">
+        <v>68</v>
+      </c>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
@@ -12975,6 +13342,9 @@
       <c r="AB27" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC27" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -13061,6 +13431,9 @@
       <c r="AB28" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC28" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -13147,6 +13520,9 @@
       <c r="AB29" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC29" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -13233,6 +13609,9 @@
       <c r="AB30" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -13319,6 +13698,9 @@
       <c r="AB31" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC31" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -13405,8 +13787,11 @@
       <c r="AB32" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC32" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -13491,8 +13876,11 @@
       <c r="AB33" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC33" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -13577,8 +13965,11 @@
       <c r="AB34" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC34" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -13663,8 +14054,11 @@
       <c r="AB35" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC35" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -13748,6 +14142,9 @@
       </c>
       <c r="AB36" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -13761,11 +14158,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A92389E-F363-478C-8FE0-DB1A38F4DB64}">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ25" sqref="B2:AJ25"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AN2" sqref="AN2:AN25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13789,9 +14186,10 @@
     <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13909,8 +14307,11 @@
       <c r="AM1" t="s">
         <v>62</v>
       </c>
+      <c r="AN1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -14028,8 +14429,11 @@
       <c r="AM2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN2" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -14147,8 +14551,11 @@
       <c r="AM3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN3" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -14266,8 +14673,11 @@
       <c r="AM4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN4" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -14385,8 +14795,11 @@
       <c r="AM5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN5" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -14504,8 +14917,11 @@
       <c r="AM6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN6" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -14623,8 +15039,11 @@
       <c r="AM7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN7" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -14742,8 +15161,11 @@
       <c r="AM8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN8" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -14861,8 +15283,11 @@
       <c r="AM9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN9" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -14980,8 +15405,11 @@
       <c r="AM10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN10" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -15099,8 +15527,11 @@
       <c r="AM11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN11" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -15218,8 +15649,11 @@
       <c r="AM12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN12" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -15337,8 +15771,11 @@
       <c r="AM13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN13" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -15456,8 +15893,11 @@
       <c r="AM14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN14" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -15575,8 +16015,11 @@
       <c r="AM15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN15" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -15694,8 +16137,11 @@
       <c r="AM16" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN16" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -15813,8 +16259,11 @@
       <c r="AM17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN17" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -15932,8 +16381,11 @@
       <c r="AM18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN18" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -16051,8 +16503,11 @@
       <c r="AM19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN19" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -16170,8 +16625,11 @@
       <c r="AM20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN20" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -16289,8 +16747,11 @@
       <c r="AM21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN21" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -16408,8 +16869,11 @@
       <c r="AM22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN22" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -16527,8 +16991,11 @@
       <c r="AM23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN23" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -16646,8 +17113,11 @@
       <c r="AM24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AN24" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -16764,6 +17234,9 @@
       </c>
       <c r="AM25" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -16780,7 +17253,7 @@
   <dimension ref="A1:AM36"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16808,6 +17281,7 @@
     <col min="24" max="24" width="11.7109375" customWidth="1"/>
     <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19.140625" customWidth="1"/>
@@ -16816,7 +17290,7 @@
     <col min="38" max="38" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -16901,8 +17375,11 @@
       <c r="AB1" t="s">
         <v>62</v>
       </c>
+      <c r="AC1" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -16987,8 +17464,11 @@
       <c r="AB2" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC2" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -17073,8 +17553,11 @@
       <c r="AB3" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC3" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -17159,8 +17642,11 @@
       <c r="AB4" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC4" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -17245,8 +17731,11 @@
       <c r="AB5" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -17331,8 +17820,11 @@
       <c r="AB6" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC6" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -17417,8 +17909,11 @@
       <c r="AB7" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -17503,8 +17998,11 @@
       <c r="AB8" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC8" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -17589,8 +18087,11 @@
       <c r="AB9" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC9" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -17675,8 +18176,11 @@
       <c r="AB10" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC10" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -17761,8 +18265,11 @@
       <c r="AB11" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC11" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -17847,8 +18354,11 @@
       <c r="AB12" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC12" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -17933,8 +18443,11 @@
       <c r="AB13" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC13" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -18019,8 +18532,11 @@
       <c r="AB14" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC14" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -18105,8 +18621,11 @@
       <c r="AB15" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC15" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -18190,6 +18709,9 @@
       </c>
       <c r="AB16" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
@@ -18277,6 +18799,9 @@
       <c r="AB17" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC17" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -18363,6 +18888,9 @@
       <c r="AB18" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC18" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -18449,6 +18977,9 @@
       <c r="AB19" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC19" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -18535,6 +19066,9 @@
       <c r="AB20" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC20" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -18621,6 +19155,9 @@
       <c r="AB21" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC21" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -18707,6 +19244,9 @@
       <c r="AB22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC22" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -18793,6 +19333,9 @@
       <c r="AB23" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC23" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -18879,6 +19422,9 @@
       <c r="AB24" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC24" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -18965,6 +19511,9 @@
       <c r="AB25" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC25" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -19051,7 +19600,9 @@
       <c r="AB26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AC26" s="1"/>
+      <c r="AC26" t="s">
+        <v>69</v>
+      </c>
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
       <c r="AF26" s="1"/>
@@ -19148,6 +19699,9 @@
       <c r="AB27" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -19234,6 +19788,9 @@
       <c r="AB28" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC28" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -19320,6 +19877,9 @@
       <c r="AB29" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC29" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -19406,6 +19966,9 @@
       <c r="AB30" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC30" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -19492,6 +20055,9 @@
       <c r="AB31" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -19578,8 +20144,11 @@
       <c r="AB32" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC32" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -19664,8 +20233,11 @@
       <c r="AB33" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC33" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -19750,8 +20322,11 @@
       <c r="AB34" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC34" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -19836,8 +20411,11 @@
       <c r="AB35" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AC35" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -19921,6 +20499,9 @@
       </c>
       <c r="AB36" s="2" t="s">
         <v>63</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>